<commit_message>
move humidity set points from code to contstruction property database
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/construction_properties.xlsx
+++ b/cea/databases/CH/archetypes/construction_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\CEAforArcGIS\cea\databases\CH\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18135" yWindow="465" windowWidth="21255" windowHeight="22020" tabRatio="785" activeTab="1"/>
+    <workbookView xWindow="18135" yWindow="465" windowWidth="21255" windowHeight="22020" tabRatio="785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5751" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5753" uniqueCount="80">
   <si>
     <t>Code</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>type_el</t>
+  </si>
+  <si>
+    <t>rhum_min_pc</t>
+  </si>
+  <si>
+    <t>rhum_max_pc</t>
   </si>
 </sst>
 </file>
@@ -12142,7 +12148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -17045,7 +17051,7 @@
         <v>T1</v>
       </c>
       <c r="F188" s="3" t="str">
-        <f>F92</f>
+        <f t="shared" ref="F188:F193" si="2">F92</f>
         <v>T1</v>
       </c>
       <c r="G188" s="3" t="str">
@@ -17074,7 +17080,7 @@
         <v>T1</v>
       </c>
       <c r="F189" s="3" t="str">
-        <f>F93</f>
+        <f t="shared" si="2"/>
         <v>T1</v>
       </c>
       <c r="G189" s="3" t="str">
@@ -17103,7 +17109,7 @@
         <v>T1</v>
       </c>
       <c r="F190" s="3" t="str">
-        <f>F94</f>
+        <f t="shared" si="2"/>
         <v>T1</v>
       </c>
       <c r="G190" s="3" t="str">
@@ -17132,7 +17138,7 @@
         <v>T1</v>
       </c>
       <c r="F191" s="3" t="str">
-        <f>F95</f>
+        <f t="shared" si="2"/>
         <v>T1</v>
       </c>
       <c r="G191" s="3" t="str">
@@ -17161,7 +17167,7 @@
         <v>T3</v>
       </c>
       <c r="F192" s="3" t="str">
-        <f>F96</f>
+        <f t="shared" si="2"/>
         <v>T3</v>
       </c>
       <c r="G192" s="3" t="str">
@@ -17190,7 +17196,7 @@
         <v>T3</v>
       </c>
       <c r="F193" s="3" t="str">
-        <f>F97</f>
+        <f t="shared" si="2"/>
         <v>T3</v>
       </c>
       <c r="G193" s="3" t="str">
@@ -24239,10 +24245,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24256,7 +24262,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -24275,8 +24281,14 @@
       <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
@@ -24295,8 +24307,14 @@
       <c r="F2" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="6">
+        <v>30</v>
+      </c>
+      <c r="H2" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -24315,8 +24333,14 @@
       <c r="F3" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="6">
+        <v>30</v>
+      </c>
+      <c r="H3" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
@@ -24332,11 +24356,17 @@
       <c r="E4" s="5">
         <v>21</v>
       </c>
-      <c r="F4" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="6">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6">
+        <v>30</v>
+      </c>
+      <c r="H4" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -24352,11 +24382,17 @@
       <c r="E5" s="5">
         <v>12</v>
       </c>
-      <c r="F5" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="6">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6">
+        <v>30</v>
+      </c>
+      <c r="H5" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
@@ -24372,11 +24408,17 @@
       <c r="E6" s="5">
         <v>12</v>
       </c>
-      <c r="F6" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="6">
+        <v>8</v>
+      </c>
+      <c r="G6" s="6">
+        <v>30</v>
+      </c>
+      <c r="H6" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -24392,11 +24434,17 @@
       <c r="E7" s="5">
         <v>12</v>
       </c>
-      <c r="F7" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="6">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6">
+        <v>30</v>
+      </c>
+      <c r="H7" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
@@ -24412,12 +24460,18 @@
       <c r="E8" s="5">
         <v>12</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="6">
         <f t="shared" ref="F8" si="0">111*0.15+10*0.85</f>
         <v>25.15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="6">
+        <v>30</v>
+      </c>
+      <c r="H8" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
@@ -24433,11 +24487,17 @@
       <c r="E9" s="5">
         <v>12</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="6">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="6">
+        <v>30</v>
+      </c>
+      <c r="H9" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>29</v>
       </c>
@@ -24453,11 +24513,17 @@
       <c r="E10" s="5">
         <v>12</v>
       </c>
-      <c r="F10" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="6">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6">
+        <v>30</v>
+      </c>
+      <c r="H10" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>30</v>
       </c>
@@ -24473,11 +24539,17 @@
       <c r="E11" s="5">
         <v>21</v>
       </c>
-      <c r="F11" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="6">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6">
+        <v>30</v>
+      </c>
+      <c r="H11" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>31</v>
       </c>
@@ -24493,11 +24565,17 @@
       <c r="E12" s="5">
         <v>12</v>
       </c>
-      <c r="F12" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="6">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6">
+        <v>30</v>
+      </c>
+      <c r="H12" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
@@ -24513,11 +24591,17 @@
       <c r="E13" s="5">
         <v>12</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="6">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="6">
+        <v>30</v>
+      </c>
+      <c r="H13" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
@@ -24533,11 +24617,17 @@
       <c r="E14" s="5">
         <v>12</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="6">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="6">
+        <v>30</v>
+      </c>
+      <c r="H14" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -24553,11 +24643,17 @@
       <c r="E15" s="5">
         <v>12</v>
       </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>30</v>
+      </c>
+      <c r="H15" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
@@ -24573,11 +24669,17 @@
       <c r="E16" s="5">
         <v>-5</v>
       </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>30</v>
+      </c>
+      <c r="H16" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>46</v>
       </c>
@@ -24593,12 +24695,18 @@
       <c r="E17" s="5">
         <v>12</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="6">
         <f>F9</f>
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="6">
+        <v>30</v>
+      </c>
+      <c r="H17" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>47</v>
       </c>
@@ -24614,11 +24722,17 @@
       <c r="E18" s="5">
         <v>12</v>
       </c>
-      <c r="F18" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="6">
+        <v>10</v>
+      </c>
+      <c r="G18" s="6">
+        <v>30</v>
+      </c>
+      <c r="H18" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
@@ -24634,8 +24748,14 @@
       <c r="E19" s="5">
         <v>12</v>
       </c>
-      <c r="F19" s="9">
-        <v>10</v>
+      <c r="F19" s="6">
+        <v>10</v>
+      </c>
+      <c r="G19" s="6">
+        <v>30</v>
+      </c>
+      <c r="H19" s="6">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor adjustments to Prakhar's data
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/construction_properties.xlsx
+++ b/cea/databases/CH/archetypes/construction_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinmo/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/archetypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1B28C6-7EAA-DE47-8B0F-6E96015D9B03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00151084-86B8-9246-88BB-6811A663C91E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19340" windowHeight="19640" tabRatio="785" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2920" windowWidth="19340" windowHeight="16460" tabRatio="785" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -894,18 +894,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -27043,7 +27032,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -27100,7 +27089,8 @@
         <v>18</v>
       </c>
       <c r="F2" s="12">
-        <v>8.3330000000000002</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G2" s="12">
         <v>30</v>
@@ -27126,7 +27116,8 @@
         <v>18</v>
       </c>
       <c r="F3" s="12">
-        <v>8.3330000000000002</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G3" s="12">
         <v>30</v>
@@ -27152,6 +27143,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="12">
+        <f>36/3.6</f>
         <v>10</v>
       </c>
       <c r="G4" s="12">
@@ -27178,7 +27170,8 @@
         <v>12</v>
       </c>
       <c r="F5" s="12">
-        <v>10.111000000000001</v>
+        <f>36/3.6</f>
+        <v>10</v>
       </c>
       <c r="G5" s="12">
         <v>30</v>
@@ -27204,7 +27197,8 @@
         <v>12</v>
       </c>
       <c r="F6" s="12">
-        <v>8.4440000000000008</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G6" s="12">
         <v>30</v>
@@ -27230,7 +27224,8 @@
         <v>12</v>
       </c>
       <c r="F7" s="12">
-        <v>8.4440000000000008</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G7" s="12">
         <v>30</v>
@@ -27256,6 +27251,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="12">
+        <f>36/3.6</f>
         <v>10</v>
       </c>
       <c r="G8" s="12">
@@ -27276,13 +27272,14 @@
         <v>18</v>
       </c>
       <c r="D9" s="3">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E9" s="5">
         <v>12</v>
       </c>
       <c r="F9" s="12">
-        <v>41.667000000000002</v>
+        <f>10*15/3.6</f>
+        <v>41.666666666666664</v>
       </c>
       <c r="G9" s="12">
         <v>30</v>
@@ -27308,7 +27305,8 @@
         <v>12</v>
       </c>
       <c r="F10" s="12">
-        <v>6.9169999999999998</v>
+        <f>25/3.6</f>
+        <v>6.9444444444444446</v>
       </c>
       <c r="G10" s="12">
         <v>30</v>
@@ -27361,6 +27359,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="12">
+        <f>9*10/3.6</f>
         <v>25</v>
       </c>
       <c r="G12" s="12">
@@ -27381,12 +27380,13 @@
         <v>24</v>
       </c>
       <c r="D13" s="3">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5">
         <v>12</v>
       </c>
       <c r="F13" s="12">
+        <f>3.6*10/3.6</f>
         <v>10</v>
       </c>
       <c r="G13" s="12">
@@ -27462,7 +27462,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="5">
-        <v>2</v>
+        <v>-18</v>
       </c>
       <c r="F16" s="12">
         <v>0</v>
@@ -27491,7 +27491,8 @@
         <v>12</v>
       </c>
       <c r="F17" s="12">
-        <v>83.332999999999998</v>
+        <f>20*15/3.6</f>
+        <v>83.333333333333329</v>
       </c>
       <c r="G17" s="12">
         <v>30</v>
@@ -27517,6 +27518,7 @@
         <v>12</v>
       </c>
       <c r="F18" s="12">
+        <f>36/3.6</f>
         <v>10</v>
       </c>
       <c r="G18" s="12">
@@ -27543,6 +27545,7 @@
         <v>12</v>
       </c>
       <c r="F19" s="12">
+        <f>36/3.6</f>
         <v>10</v>
       </c>
       <c r="G19" s="12">
@@ -27569,7 +27572,8 @@
         <v>12</v>
       </c>
       <c r="F20" s="12">
-        <v>8.3330000000000002</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G20" s="12">
         <v>30</v>
@@ -27589,7 +27593,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -27810,6 +27814,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="14">
+        <f>9.3+24</f>
         <v>33.299999999999997</v>
       </c>
       <c r="F6" s="14">
@@ -27845,9 +27850,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="14">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E7" s="14">
+        <f>9.3+12</f>
         <v>21.3</v>
       </c>
       <c r="F7" s="14">
@@ -27863,7 +27869,7 @@
         <v>30</v>
       </c>
       <c r="J7" s="12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K7" s="12">
         <v>0</v>
@@ -28380,12 +28386,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28559,15 +28562,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28591,17 +28605,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding occupancy type to data helper
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/construction_properties.xlsx
+++ b/cea/databases/CH/archetypes/construction_properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6075" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6076" uniqueCount="80">
   <si>
     <t>Code</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Qcpro_Wm2</t>
+  </si>
+  <si>
+    <t>Occ_m2pax</t>
   </si>
 </sst>
 </file>
@@ -27014,7 +27017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -27334,555 +27337,596 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="12" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="13">
+        <v>30</v>
+      </c>
+      <c r="C2" s="13">
         <v>70</v>
       </c>
-      <c r="C2" s="13">
+      <c r="D2" s="13">
         <v>80</v>
       </c>
-      <c r="D2" s="13">
-        <v>8</v>
-      </c>
       <c r="E2" s="13">
+        <v>8</v>
+      </c>
+      <c r="F2" s="13">
         <v>2.7</v>
       </c>
-      <c r="F2" s="11">
-        <v>0</v>
-      </c>
       <c r="G2" s="11">
         <v>0</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13">
         <v>35</v>
       </c>
-      <c r="I2" s="13">
+      <c r="J2" s="13">
         <v>140</v>
       </c>
-      <c r="J2" s="11">
-        <v>0</v>
-      </c>
       <c r="K2" s="11">
         <v>0</v>
       </c>
       <c r="L2" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="13">
+        <v>50</v>
+      </c>
+      <c r="C3" s="11">
         <v>70</v>
       </c>
-      <c r="C3" s="11">
+      <c r="D3" s="11">
         <v>80</v>
       </c>
-      <c r="D3" s="11">
-        <v>8</v>
-      </c>
       <c r="E3" s="11">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11">
         <v>2.7</v>
       </c>
-      <c r="F3" s="13">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="13">
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
         <v>40</v>
       </c>
-      <c r="I3" s="13">
+      <c r="J3" s="13">
         <v>160</v>
       </c>
-      <c r="J3" s="11">
-        <v>0</v>
-      </c>
       <c r="K3" s="11">
         <v>0</v>
       </c>
       <c r="L3" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="13">
+        <v>15</v>
+      </c>
+      <c r="C4" s="13">
         <v>70</v>
       </c>
-      <c r="C4" s="13">
+      <c r="D4" s="13">
         <v>80</v>
       </c>
-      <c r="D4" s="13">
-        <v>8</v>
-      </c>
       <c r="E4" s="13">
+        <v>8</v>
+      </c>
+      <c r="F4" s="13">
         <v>2.7</v>
       </c>
-      <c r="F4" s="13">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-      <c r="H4" s="13">
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
         <v>40</v>
       </c>
-      <c r="I4" s="13">
+      <c r="J4" s="13">
         <v>160</v>
       </c>
-      <c r="J4" s="11">
-        <v>0</v>
-      </c>
       <c r="K4" s="11">
         <v>0</v>
       </c>
       <c r="L4" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="13">
+        <v>14</v>
+      </c>
+      <c r="C5" s="13">
         <v>70</v>
       </c>
-      <c r="C5" s="13">
+      <c r="D5" s="13">
         <v>80</v>
       </c>
-      <c r="D5" s="13">
-        <v>7</v>
-      </c>
       <c r="E5" s="13">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13">
         <v>15.9</v>
       </c>
-      <c r="F5" s="13">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
-        <v>0</v>
-      </c>
-      <c r="H5" s="13">
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13">
         <v>3</v>
       </c>
-      <c r="I5" s="13">
+      <c r="J5" s="13">
         <v>60</v>
       </c>
-      <c r="J5" s="11">
-        <v>0</v>
-      </c>
       <c r="K5" s="11">
         <v>0</v>
       </c>
       <c r="L5" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="13">
+        <v>8</v>
+      </c>
+      <c r="C6" s="13">
         <v>70</v>
       </c>
-      <c r="C6" s="13">
+      <c r="D6" s="13">
         <v>80</v>
       </c>
-      <c r="D6" s="13">
+      <c r="E6" s="13">
         <v>2</v>
       </c>
-      <c r="E6" s="13">
+      <c r="F6" s="13">
         <f>9.3+24</f>
         <v>33.299999999999997</v>
       </c>
-      <c r="F6" s="13">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0</v>
-      </c>
-      <c r="H6" s="13">
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
         <v>2</v>
       </c>
-      <c r="I6" s="13">
+      <c r="J6" s="13">
         <v>30</v>
       </c>
-      <c r="J6" s="11">
-        <v>0</v>
-      </c>
       <c r="K6" s="11">
         <v>0</v>
       </c>
       <c r="L6" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="13">
+        <v>8</v>
+      </c>
+      <c r="C7" s="13">
         <v>70</v>
       </c>
-      <c r="C7" s="13">
+      <c r="D7" s="13">
         <v>80</v>
       </c>
-      <c r="D7" s="13">
+      <c r="E7" s="13">
         <v>2</v>
       </c>
-      <c r="E7" s="13">
+      <c r="F7" s="13">
         <f>9.3+12</f>
         <v>21.3</v>
       </c>
-      <c r="F7" s="13">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
         <v>2</v>
       </c>
-      <c r="I7" s="13">
+      <c r="J7" s="13">
         <v>30</v>
       </c>
-      <c r="J7" s="11">
-        <v>10</v>
-      </c>
       <c r="K7" s="11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L7" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="13">
+        <v>2</v>
+      </c>
+      <c r="C8" s="13">
         <v>70</v>
       </c>
-      <c r="C8" s="13">
+      <c r="D8" s="13">
         <v>80</v>
       </c>
-      <c r="D8" s="13">
+      <c r="E8" s="13">
         <v>2</v>
       </c>
-      <c r="E8" s="13">
+      <c r="F8" s="13">
         <v>6.9</v>
       </c>
-      <c r="F8" s="13">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="13">
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
         <v>15</v>
       </c>
-      <c r="I8" s="13">
+      <c r="J8" s="13">
         <v>45</v>
       </c>
-      <c r="J8" s="11">
-        <v>0</v>
-      </c>
       <c r="K8" s="11">
         <v>0</v>
       </c>
       <c r="L8" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="13">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13">
         <v>90</v>
       </c>
-      <c r="C9" s="13">
+      <c r="D9" s="13">
         <v>170</v>
       </c>
-      <c r="D9" s="13">
-        <v>10</v>
-      </c>
       <c r="E9" s="13">
+        <v>10</v>
+      </c>
+      <c r="F9" s="13">
         <v>10.8</v>
       </c>
-      <c r="F9" s="13">
+      <c r="G9" s="13">
         <v>16.5</v>
       </c>
-      <c r="G9" s="11">
-        <v>0</v>
-      </c>
-      <c r="H9" s="13">
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
         <v>3</v>
       </c>
-      <c r="I9" s="13">
+      <c r="J9" s="13">
         <v>60</v>
       </c>
-      <c r="J9" s="11">
-        <v>0</v>
-      </c>
       <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
         <v>150</v>
       </c>
-      <c r="L9" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="13">
+        <v>3</v>
+      </c>
+      <c r="C10" s="13">
         <v>70</v>
       </c>
-      <c r="C10" s="13">
+      <c r="D10" s="13">
         <v>80</v>
       </c>
-      <c r="D10" s="13">
+      <c r="E10" s="13">
         <v>4</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="13">
         <v>14</v>
       </c>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="11">
-        <v>0</v>
-      </c>
-      <c r="H10" s="13">
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
         <v>2</v>
       </c>
-      <c r="I10" s="13">
+      <c r="J10" s="13">
         <v>30</v>
       </c>
-      <c r="J10" s="11">
-        <v>0</v>
-      </c>
       <c r="K10" s="11">
         <v>0</v>
       </c>
       <c r="L10" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="13">
+        <f>15*0.43+3*0.01+5*0.56</f>
+        <v>9.2800000000000011</v>
+      </c>
+      <c r="C11" s="13">
         <v>70</v>
       </c>
-      <c r="C11" s="13">
+      <c r="D11" s="13">
         <v>80</v>
       </c>
-      <c r="D11" s="13">
+      <c r="E11" s="13">
         <f>0.43*4+0.01*7+0.56*20</f>
         <v>12.990000000000002</v>
       </c>
-      <c r="E11" s="13">
+      <c r="F11" s="13">
         <f>0.43*4.5+0.01*15.9+0.56*15.9</f>
         <v>10.998000000000001</v>
       </c>
-      <c r="F11" s="13">
-        <v>0</v>
-      </c>
-      <c r="G11" s="11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="13">
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
         <f>0.43*60+0.01*0+0.56*0</f>
         <v>25.8</v>
       </c>
-      <c r="I11" s="13">
-        <f>H11*4</f>
+      <c r="J11" s="13">
+        <f>I11*4</f>
         <v>103.2</v>
       </c>
-      <c r="J11" s="11">
-        <v>0</v>
-      </c>
       <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11">
         <v>16</v>
       </c>
-      <c r="L11" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="13">
+        <v>10</v>
+      </c>
+      <c r="C12" s="13">
         <v>120</v>
       </c>
-      <c r="C12" s="13">
+      <c r="D12" s="13">
         <v>280</v>
       </c>
-      <c r="D12" s="13">
+      <c r="E12" s="13">
         <v>2</v>
       </c>
-      <c r="E12" s="13">
+      <c r="F12" s="13">
         <v>9.9</v>
       </c>
-      <c r="F12" s="13">
-        <v>0</v>
-      </c>
-      <c r="G12" s="11">
-        <v>0</v>
-      </c>
-      <c r="H12" s="13">
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
         <v>60</v>
       </c>
-      <c r="I12" s="13">
+      <c r="J12" s="13">
         <v>180</v>
       </c>
-      <c r="J12" s="11">
-        <v>0</v>
-      </c>
       <c r="K12" s="11">
         <v>0</v>
       </c>
       <c r="L12" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="13">
         <v>70</v>
       </c>
-      <c r="C13" s="13">
+      <c r="D13" s="13">
         <v>80</v>
       </c>
-      <c r="D13" s="13">
+      <c r="E13" s="13">
         <v>2</v>
       </c>
-      <c r="E13" s="13">
+      <c r="F13" s="13">
         <v>11.3</v>
       </c>
-      <c r="F13" s="13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="11">
-        <v>0</v>
-      </c>
-      <c r="H13" s="13">
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
         <v>120</v>
       </c>
-      <c r="I13" s="13">
+      <c r="J13" s="13">
         <v>360</v>
       </c>
-      <c r="J13" s="11">
-        <v>0</v>
-      </c>
       <c r="K13" s="11">
         <v>0</v>
       </c>
       <c r="L13" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="13">
+        <v>0</v>
+      </c>
+      <c r="C14" s="13">
         <v>70</v>
       </c>
-      <c r="C14" s="13">
-        <v>0</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0</v>
-      </c>
-      <c r="E14" s="13">
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
         <v>6.6</v>
       </c>
-      <c r="F14" s="13">
-        <v>0</v>
-      </c>
       <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
         <v>100</v>
       </c>
-      <c r="H14" s="13">
-        <v>0</v>
-      </c>
       <c r="I14" s="13">
         <v>0</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="13">
         <v>0</v>
       </c>
       <c r="K14" s="11">
@@ -27891,36 +27935,39 @@
       <c r="L14" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="13">
+        <v>0</v>
+      </c>
+      <c r="C15" s="13">
         <v>35</v>
       </c>
-      <c r="C15" s="13">
-        <v>0</v>
-      </c>
       <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
         <v>1</v>
       </c>
-      <c r="E15" s="13">
+      <c r="F15" s="13">
         <v>2.9</v>
       </c>
-      <c r="F15" s="13">
-        <v>0</v>
-      </c>
-      <c r="G15" s="11">
-        <v>0</v>
-      </c>
-      <c r="H15" s="13">
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
         <v>0</v>
       </c>
       <c r="I15" s="13">
         <v>0</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="13">
         <v>0</v>
       </c>
       <c r="K15" s="11">
@@ -27929,153 +27976,165 @@
       <c r="L15" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="13">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
         <v>70</v>
       </c>
-      <c r="C16" s="13">
-        <v>0</v>
-      </c>
       <c r="D16" s="13">
         <v>0</v>
       </c>
       <c r="E16" s="13">
+        <v>0</v>
+      </c>
+      <c r="F16" s="13">
         <v>5.7</v>
       </c>
-      <c r="F16" s="13">
-        <v>0</v>
-      </c>
-      <c r="G16" s="11">
-        <v>0</v>
-      </c>
-      <c r="H16" s="13">
+      <c r="G16" s="13">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
         <v>0</v>
       </c>
       <c r="I16" s="13">
         <v>0</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="11">
         <v>100</v>
       </c>
-      <c r="K16" s="11">
-        <v>0</v>
-      </c>
       <c r="L16" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="13">
-        <f>B11</f>
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C17" s="13">
         <f>C11</f>
+        <v>70</v>
+      </c>
+      <c r="D17" s="13">
+        <f>D11</f>
         <v>80</v>
       </c>
-      <c r="D17" s="13">
+      <c r="E17" s="13">
         <v>20</v>
       </c>
-      <c r="E17" s="13">
+      <c r="F17" s="13">
         <v>16.2</v>
       </c>
-      <c r="F17" s="13">
-        <f>F9</f>
+      <c r="G17" s="13">
+        <f>G9</f>
         <v>16.5</v>
       </c>
-      <c r="G17" s="11">
-        <v>0</v>
-      </c>
-      <c r="H17" s="13">
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="13">
         <v>3</v>
       </c>
-      <c r="I17" s="13">
+      <c r="J17" s="13">
         <v>60</v>
       </c>
-      <c r="J17" s="11">
-        <v>0</v>
-      </c>
       <c r="K17" s="11">
         <v>0</v>
       </c>
       <c r="L17" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="13">
+        <v>3</v>
+      </c>
+      <c r="C18" s="13">
         <v>70</v>
       </c>
-      <c r="C18" s="13">
+      <c r="D18" s="13">
         <v>80</v>
       </c>
-      <c r="D18" s="13">
-        <v>7</v>
-      </c>
       <c r="E18" s="13">
+        <v>7</v>
+      </c>
+      <c r="F18" s="13">
         <v>10.8</v>
       </c>
-      <c r="F18" s="13">
-        <v>0</v>
-      </c>
-      <c r="G18" s="11">
-        <v>0</v>
-      </c>
-      <c r="H18" s="13">
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="13">
         <v>2</v>
       </c>
-      <c r="I18" s="13">
+      <c r="J18" s="13">
         <v>30</v>
       </c>
-      <c r="J18" s="11">
-        <v>0</v>
-      </c>
       <c r="K18" s="11">
         <v>0</v>
       </c>
       <c r="L18" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="13">
+        <v>5</v>
+      </c>
+      <c r="C19" s="13">
         <v>70</v>
       </c>
-      <c r="C19" s="13">
+      <c r="D19" s="13">
         <v>80</v>
       </c>
-      <c r="D19" s="13">
+      <c r="E19" s="13">
         <v>2</v>
       </c>
-      <c r="E19" s="13">
+      <c r="F19" s="13">
         <v>6.9</v>
       </c>
-      <c r="F19" s="13">
-        <v>0</v>
-      </c>
-      <c r="G19" s="11">
-        <v>0</v>
-      </c>
-      <c r="H19" s="13">
+      <c r="G19" s="13">
+        <v>0</v>
+      </c>
+      <c r="H19" s="11">
         <v>0</v>
       </c>
       <c r="I19" s="13">
         <v>0</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="13">
         <v>0</v>
       </c>
       <c r="K19" s="11">
@@ -28084,42 +28143,48 @@
       <c r="L19" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="13">
+        <v>10</v>
+      </c>
+      <c r="C20" s="13">
         <v>70</v>
       </c>
-      <c r="C20" s="13">
+      <c r="D20" s="13">
         <v>80</v>
       </c>
-      <c r="D20" s="13">
+      <c r="E20" s="13">
         <v>4</v>
       </c>
-      <c r="E20" s="13">
+      <c r="F20" s="13">
         <v>12.5</v>
       </c>
-      <c r="F20" s="13">
-        <v>0</v>
-      </c>
-      <c r="G20" s="11">
-        <v>0</v>
-      </c>
-      <c r="H20" s="13">
+      <c r="G20" s="13">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="13">
         <v>2</v>
       </c>
-      <c r="I20" s="13">
+      <c r="J20" s="13">
         <v>30</v>
       </c>
-      <c r="J20" s="11">
-        <v>0</v>
-      </c>
       <c r="K20" s="11">
         <v>0</v>
       </c>
       <c r="L20" s="11">
+        <v>0</v>
+      </c>
+      <c r="M20" s="11">
         <v>0</v>
       </c>
     </row>
@@ -28130,12 +28195,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28309,15 +28371,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28341,17 +28414,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
hotfix archetypes variables names
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/construction_properties.xlsx
+++ b/cea/databases/CH/archetypes/construction_properties.xlsx
@@ -246,12 +246,6 @@
     <t>type_el</t>
   </si>
   <si>
-    <t>rhum_min_pc</t>
-  </si>
-  <si>
-    <t>rhum_max_pc</t>
-  </si>
-  <si>
     <t>Qcre_Wm2</t>
   </si>
   <si>
@@ -283,6 +277,12 @@
   </si>
   <si>
     <t>Ve_lpspax</t>
+  </si>
+  <si>
+    <t>RH_min_pc</t>
+  </si>
+  <si>
+    <t>RH_max_pc</t>
   </si>
 </sst>
 </file>
@@ -1304,13 +1304,13 @@
         <v>62</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>69</v>
@@ -13592,7 +13592,7 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B218" s="6">
         <v>1000</v>
@@ -13648,7 +13648,7 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>47</v>
@@ -13704,7 +13704,7 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>48</v>
@@ -13760,7 +13760,7 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B221" s="6" t="s">
         <v>49</v>
@@ -13816,7 +13816,7 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B222" s="6" t="s">
         <v>55</v>
@@ -13872,7 +13872,7 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B223" s="6" t="s">
         <v>56</v>
@@ -13928,7 +13928,7 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B224" s="6">
         <v>1000</v>
@@ -13984,7 +13984,7 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B225" s="6" t="s">
         <v>47</v>
@@ -14040,7 +14040,7 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B226" s="6" t="s">
         <v>48</v>
@@ -14096,7 +14096,7 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B227" s="6" t="s">
         <v>49</v>
@@ -14152,7 +14152,7 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B228" s="6" t="s">
         <v>55</v>
@@ -14208,7 +14208,7 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B229" s="6" t="s">
         <v>56</v>
@@ -19959,7 +19959,7 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B218" s="6" t="s">
         <v>57</v>
@@ -19985,7 +19985,7 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>47</v>
@@ -20011,7 +20011,7 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>48</v>
@@ -20037,7 +20037,7 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B221" s="6" t="s">
         <v>49</v>
@@ -20063,7 +20063,7 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B222" s="6" t="s">
         <v>55</v>
@@ -20089,7 +20089,7 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B223" s="6" t="s">
         <v>56</v>
@@ -20115,7 +20115,7 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>57</v>
@@ -20141,7 +20141,7 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B225" s="6" t="s">
         <v>47</v>
@@ -20167,7 +20167,7 @@
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B226" s="6" t="s">
         <v>48</v>
@@ -20193,7 +20193,7 @@
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B227" s="6" t="s">
         <v>49</v>
@@ -20219,7 +20219,7 @@
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B228" s="6" t="s">
         <v>55</v>
@@ -20245,7 +20245,7 @@
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B229" s="6" t="s">
         <v>56</v>
@@ -26677,7 +26677,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B218" s="6" t="s">
         <v>57</v>
@@ -26706,7 +26706,7 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>47</v>
@@ -26735,7 +26735,7 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>48</v>
@@ -26764,7 +26764,7 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B221" s="6" t="s">
         <v>49</v>
@@ -26793,7 +26793,7 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B222" s="6" t="s">
         <v>55</v>
@@ -26822,7 +26822,7 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B223" s="6" t="s">
         <v>56</v>
@@ -26851,7 +26851,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>57</v>
@@ -26880,7 +26880,7 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B225" s="6" t="s">
         <v>47</v>
@@ -26909,7 +26909,7 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B226" s="6" t="s">
         <v>48</v>
@@ -26938,7 +26938,7 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B227" s="6" t="s">
         <v>49</v>
@@ -26967,7 +26967,7 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B228" s="6" t="s">
         <v>55</v>
@@ -26996,7 +26996,7 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B229" s="6" t="s">
         <v>56</v>
@@ -27034,7 +27034,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27065,13 +27065,13 @@
         <v>34</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -27559,7 +27559,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B20" s="3">
         <v>26</v>
@@ -27622,13 +27622,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>13</v>
@@ -27643,19 +27643,19 @@
         <v>32</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -28408,7 +28408,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B20" s="14">
         <v>10</v>
@@ -28454,9 +28454,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28630,26 +28633,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28673,9 +28665,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
simplifying databases and fixing input locator
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/construction_properties.xlsx
+++ b/cea/databases/CH/archetypes/construction_properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6080" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6080" uniqueCount="87">
   <si>
     <t>Code</t>
   </si>
@@ -283,6 +283,15 @@
   </si>
   <si>
     <t>RH_max_pc</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>T24</t>
   </si>
 </sst>
 </file>
@@ -14275,8 +14284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K224" sqref="K224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14340,7 +14349,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -14366,7 +14375,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -14392,7 +14401,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -14418,7 +14427,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -14444,7 +14453,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -14470,7 +14479,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -14496,7 +14505,7 @@
         <v>9</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -14522,7 +14531,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -14548,7 +14557,7 @@
         <v>9</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -14574,7 +14583,7 @@
         <v>9</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -14600,7 +14609,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -14626,7 +14635,7 @@
         <v>9</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -14652,7 +14661,7 @@
         <v>9</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -14678,7 +14687,7 @@
         <v>9</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -14704,7 +14713,7 @@
         <v>9</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -14730,7 +14739,7 @@
         <v>9</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -14756,7 +14765,7 @@
         <v>9</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -14782,7 +14791,7 @@
         <v>9</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -14808,7 +14817,7 @@
         <v>9</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -14834,7 +14843,7 @@
         <v>9</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -14860,7 +14869,7 @@
         <v>9</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -14886,7 +14895,7 @@
         <v>9</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -14909,10 +14918,10 @@
         <v>7</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -14935,10 +14944,10 @@
         <v>7</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -14964,7 +14973,7 @@
         <v>9</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -14987,10 +14996,10 @@
         <v>8</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -15013,10 +15022,10 @@
         <v>8</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -15039,10 +15048,10 @@
         <v>8</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -15065,10 +15074,10 @@
         <v>10</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -15091,10 +15100,10 @@
         <v>10</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -15117,10 +15126,10 @@
         <v>8</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -15143,10 +15152,10 @@
         <v>8</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -15169,10 +15178,10 @@
         <v>8</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -15195,10 +15204,10 @@
         <v>8</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -15221,10 +15230,10 @@
         <v>10</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -15247,10 +15256,10 @@
         <v>10</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -15276,7 +15285,7 @@
         <v>9</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -15299,10 +15308,10 @@
         <v>8</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -15325,10 +15334,10 @@
         <v>8</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -15351,10 +15360,10 @@
         <v>8</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -15377,10 +15386,10 @@
         <v>7</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -15403,10 +15412,10 @@
         <v>7</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -15429,10 +15438,10 @@
         <v>8</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -15455,10 +15464,10 @@
         <v>8</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -15481,10 +15490,10 @@
         <v>8</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -15507,10 +15516,10 @@
         <v>8</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -15533,10 +15542,10 @@
         <v>7</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -15559,10 +15568,10 @@
         <v>7</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -15588,7 +15597,7 @@
         <v>9</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -15611,10 +15620,10 @@
         <v>8</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -15637,10 +15646,10 @@
         <v>8</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -15663,10 +15672,10 @@
         <v>8</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -15689,10 +15698,10 @@
         <v>7</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -15715,10 +15724,10 @@
         <v>7</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -15741,10 +15750,10 @@
         <v>8</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -15767,10 +15776,10 @@
         <v>8</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -15793,10 +15802,10 @@
         <v>8</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -15819,10 +15828,10 @@
         <v>8</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -15845,10 +15854,10 @@
         <v>7</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -15871,10 +15880,10 @@
         <v>7</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -15900,7 +15909,7 @@
         <v>9</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -15923,10 +15932,10 @@
         <v>8</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -15949,10 +15958,10 @@
         <v>8</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -15975,10 +15984,10 @@
         <v>8</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -16001,10 +16010,10 @@
         <v>7</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -16027,10 +16036,10 @@
         <v>7</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -16053,10 +16062,10 @@
         <v>8</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -16079,10 +16088,10 @@
         <v>8</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -16105,10 +16114,10 @@
         <v>8</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -16131,10 +16140,10 @@
         <v>8</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -16157,10 +16166,10 @@
         <v>7</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -16183,10 +16192,10 @@
         <v>7</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -16212,7 +16221,7 @@
         <v>9</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -16235,10 +16244,10 @@
         <v>8</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -16261,10 +16270,10 @@
         <v>8</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -16287,10 +16296,10 @@
         <v>8</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -16313,10 +16322,10 @@
         <v>7</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -16339,10 +16348,10 @@
         <v>7</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -16365,10 +16374,10 @@
         <v>8</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -16391,10 +16400,10 @@
         <v>8</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -16417,10 +16426,10 @@
         <v>8</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -16443,10 +16452,10 @@
         <v>8</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -16469,10 +16478,10 @@
         <v>7</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -16495,10 +16504,10 @@
         <v>7</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -16521,10 +16530,10 @@
         <v>8</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -16547,10 +16556,10 @@
         <v>8</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -16573,10 +16582,10 @@
         <v>8</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -16599,10 +16608,10 @@
         <v>8</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -16625,10 +16634,10 @@
         <v>7</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -16651,10 +16660,10 @@
         <v>7</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -16677,10 +16686,10 @@
         <v>8</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -16703,10 +16712,10 @@
         <v>8</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -16729,10 +16738,10 @@
         <v>8</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -16755,10 +16764,10 @@
         <v>8</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -16781,10 +16790,10 @@
         <v>7</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -16807,10 +16816,10 @@
         <v>7</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -16836,7 +16845,7 @@
         <v>9</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -16859,10 +16868,10 @@
         <v>8</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -16885,10 +16894,10 @@
         <v>8</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -16911,10 +16920,10 @@
         <v>8</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -16937,10 +16946,10 @@
         <v>7</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -16963,10 +16972,10 @@
         <v>7</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -16989,10 +16998,10 @@
         <v>8</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -17015,10 +17024,10 @@
         <v>8</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -17041,10 +17050,10 @@
         <v>8</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -17067,10 +17076,10 @@
         <v>7</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -17093,10 +17102,10 @@
         <v>7</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -17119,10 +17128,10 @@
         <v>7</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -17148,7 +17157,7 @@
         <v>9</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -17171,10 +17180,10 @@
         <v>8</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -17197,10 +17206,10 @@
         <v>8</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -17223,10 +17232,10 @@
         <v>8</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -17249,10 +17258,10 @@
         <v>7</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -17275,10 +17284,10 @@
         <v>7</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -17301,10 +17310,10 @@
         <v>8</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -17327,10 +17336,10 @@
         <v>8</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -17353,10 +17362,10 @@
         <v>8</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -17379,10 +17388,10 @@
         <v>7</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -17405,10 +17414,10 @@
         <v>7</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -17431,10 +17440,10 @@
         <v>7</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -17460,7 +17469,7 @@
         <v>9</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -17483,10 +17492,10 @@
         <v>8</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -17509,10 +17518,10 @@
         <v>7</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -17535,10 +17544,10 @@
         <v>7</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -17561,10 +17570,10 @@
         <v>7</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -17587,10 +17596,10 @@
         <v>7</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -17613,10 +17622,10 @@
         <v>7</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -17639,10 +17648,10 @@
         <v>7</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -17665,10 +17674,10 @@
         <v>7</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -17691,10 +17700,10 @@
         <v>7</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -17717,10 +17726,10 @@
         <v>7</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -17743,10 +17752,10 @@
         <v>7</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -17772,7 +17781,7 @@
         <v>9</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -17798,7 +17807,7 @@
         <v>9</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -17824,7 +17833,7 @@
         <v>9</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -17850,7 +17859,7 @@
         <v>9</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -17876,7 +17885,7 @@
         <v>9</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -17902,7 +17911,7 @@
         <v>9</v>
       </c>
       <c r="H139" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -17928,7 +17937,7 @@
         <v>9</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -17954,7 +17963,7 @@
         <v>9</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -17980,7 +17989,7 @@
         <v>9</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -18006,7 +18015,7 @@
         <v>9</v>
       </c>
       <c r="H143" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -18032,7 +18041,7 @@
         <v>9</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -18058,7 +18067,7 @@
         <v>9</v>
       </c>
       <c r="H145" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -18081,10 +18090,10 @@
         <v>9</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -18107,10 +18116,10 @@
         <v>9</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -18133,10 +18142,10 @@
         <v>9</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -18159,10 +18168,10 @@
         <v>9</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -18185,10 +18194,10 @@
         <v>9</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -18211,10 +18220,10 @@
         <v>9</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -18237,10 +18246,10 @@
         <v>9</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -18263,10 +18272,10 @@
         <v>9</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -18289,10 +18298,10 @@
         <v>9</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H154" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -18315,10 +18324,10 @@
         <v>9</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -18341,10 +18350,10 @@
         <v>9</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H156" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -18367,10 +18376,10 @@
         <v>9</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H157" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -18396,7 +18405,7 @@
         <v>9</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -18422,7 +18431,7 @@
         <v>9</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -18448,7 +18457,7 @@
         <v>9</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -18474,7 +18483,7 @@
         <v>9</v>
       </c>
       <c r="H161" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -18500,7 +18509,7 @@
         <v>9</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -18526,7 +18535,7 @@
         <v>9</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -18552,7 +18561,7 @@
         <v>9</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -18578,7 +18587,7 @@
         <v>9</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -18604,7 +18613,7 @@
         <v>9</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -18630,7 +18639,7 @@
         <v>9</v>
       </c>
       <c r="H167" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -18656,7 +18665,7 @@
         <v>9</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -18682,7 +18691,7 @@
         <v>9</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -18705,10 +18714,10 @@
         <v>9</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -18731,10 +18740,10 @@
         <v>9</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H171" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -18757,10 +18766,10 @@
         <v>9</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -18783,10 +18792,10 @@
         <v>9</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -18809,10 +18818,10 @@
         <v>9</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -18835,10 +18844,10 @@
         <v>9</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H175" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -18861,10 +18870,10 @@
         <v>9</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H176" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -18887,10 +18896,10 @@
         <v>9</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -18913,10 +18922,10 @@
         <v>9</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -18939,10 +18948,10 @@
         <v>9</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H179" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -18965,10 +18974,10 @@
         <v>9</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H180" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -18991,10 +19000,10 @@
         <v>9</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -19021,7 +19030,7 @@
         <v>T0</v>
       </c>
       <c r="H182" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -19045,10 +19054,10 @@
       </c>
       <c r="G183" s="3" t="str">
         <f t="shared" ref="G183:G193" si="0">G99</f>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H183" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -19072,10 +19081,10 @@
       </c>
       <c r="G184" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H184" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -19099,10 +19108,10 @@
       </c>
       <c r="G185" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H185" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
@@ -19126,10 +19135,10 @@
       </c>
       <c r="G186" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -19153,10 +19162,10 @@
       </c>
       <c r="G187" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H187" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -19182,10 +19191,10 @@
       </c>
       <c r="G188" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H188" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
@@ -19211,10 +19220,10 @@
       </c>
       <c r="G189" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H189" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -19240,10 +19249,10 @@
       </c>
       <c r="G190" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H190" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -19269,10 +19278,10 @@
       </c>
       <c r="G191" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H191" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
@@ -19298,10 +19307,10 @@
       </c>
       <c r="G192" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H192" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -19327,10 +19336,10 @@
       </c>
       <c r="G193" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>T3</v>
+        <v>T19</v>
       </c>
       <c r="H193" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -19356,7 +19365,7 @@
         <v>9</v>
       </c>
       <c r="H194" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -19379,10 +19388,10 @@
         <v>8</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H195" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -19405,10 +19414,10 @@
         <v>8</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H196" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -19431,10 +19440,10 @@
         <v>8</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H197" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
@@ -19457,10 +19466,10 @@
         <v>7</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H198" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -19483,10 +19492,10 @@
         <v>7</v>
       </c>
       <c r="G199" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H199" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
@@ -19509,10 +19518,10 @@
         <v>8</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H200" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
@@ -19535,10 +19544,10 @@
         <v>8</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H201" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -19561,10 +19570,10 @@
         <v>8</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H202" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -19587,10 +19596,10 @@
         <v>7</v>
       </c>
       <c r="G203" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H203" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
@@ -19613,10 +19622,10 @@
         <v>7</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H204" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
@@ -19639,10 +19648,10 @@
         <v>7</v>
       </c>
       <c r="G205" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H205" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
@@ -19668,7 +19677,7 @@
         <v>9</v>
       </c>
       <c r="H206" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
@@ -19691,10 +19700,10 @@
         <v>8</v>
       </c>
       <c r="G207" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H207" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
@@ -19717,10 +19726,10 @@
         <v>8</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H208" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
@@ -19743,10 +19752,10 @@
         <v>8</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H209" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
@@ -19769,10 +19778,10 @@
         <v>7</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H210" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
@@ -19795,10 +19804,10 @@
         <v>7</v>
       </c>
       <c r="G211" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H211" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -19821,10 +19830,10 @@
         <v>8</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H212" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -19847,10 +19856,10 @@
         <v>8</v>
       </c>
       <c r="G213" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H213" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -19873,10 +19882,10 @@
         <v>8</v>
       </c>
       <c r="G214" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H214" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -19899,10 +19908,10 @@
         <v>7</v>
       </c>
       <c r="G215" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H215" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -19925,10 +19934,10 @@
         <v>7</v>
       </c>
       <c r="G216" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H216" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -19951,10 +19960,10 @@
         <v>7</v>
       </c>
       <c r="G217" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H217" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -19980,7 +19989,7 @@
         <v>9</v>
       </c>
       <c r="H218" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -20003,10 +20012,10 @@
         <v>8</v>
       </c>
       <c r="G219" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H219" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -20029,10 +20038,10 @@
         <v>8</v>
       </c>
       <c r="G220" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H220" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -20055,10 +20064,10 @@
         <v>8</v>
       </c>
       <c r="G221" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H221" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -20081,10 +20090,10 @@
         <v>7</v>
       </c>
       <c r="G222" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H222" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -20107,10 +20116,10 @@
         <v>7</v>
       </c>
       <c r="G223" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H223" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -20133,10 +20142,10 @@
         <v>8</v>
       </c>
       <c r="G224" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H224" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -20159,10 +20168,10 @@
         <v>8</v>
       </c>
       <c r="G225" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H225" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
@@ -20185,10 +20194,10 @@
         <v>8</v>
       </c>
       <c r="G226" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H226" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
@@ -20211,10 +20220,10 @@
         <v>7</v>
       </c>
       <c r="G227" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H227" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
@@ -20237,10 +20246,10 @@
         <v>7</v>
       </c>
       <c r="G228" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H228" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -20263,10 +20272,10 @@
         <v>7</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H229" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -27033,7 +27042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -28454,15 +28463,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -28632,6 +28632,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -28639,14 +28648,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28660,6 +28661,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update archetypes to include economizers
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/construction_properties.xlsx
+++ b/cea/databases/CH/archetypes/construction_properties.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Assistenz\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
@@ -1271,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E203" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12068,7 +12068,7 @@
         <v>0</v>
       </c>
       <c r="H183" s="3">
-        <f t="shared" ref="G183:H193" si="2">H87</f>
+        <f t="shared" ref="H183:H193" si="2">H87</f>
         <v>0.9</v>
       </c>
       <c r="I183" s="11">
@@ -12805,7 +12805,7 @@
         <v>0</v>
       </c>
       <c r="H194" s="3">
-        <f t="shared" ref="G194:H205" si="16">H182</f>
+        <f t="shared" ref="H194:H205" si="16">H182</f>
         <v>0.9</v>
       </c>
       <c r="I194" s="11">
@@ -14965,8 +14965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20968,11 +20968,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I229"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E124" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F134" sqref="F134"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21188,7 +21188,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -21536,7 +21536,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -21855,7 +21855,7 @@
         <v>9</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -21884,7 +21884,7 @@
         <v>6</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -22029,7 +22029,7 @@
         <v>9</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -22058,7 +22058,7 @@
         <v>6</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -22203,7 +22203,7 @@
         <v>9</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -22232,7 +22232,7 @@
         <v>6</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -22377,7 +22377,7 @@
         <v>9</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -22406,7 +22406,7 @@
         <v>6</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -22551,7 +22551,7 @@
         <v>9</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -22580,7 +22580,7 @@
         <v>6</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -22725,7 +22725,7 @@
         <v>9</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -22754,7 +22754,7 @@
         <v>6</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -22899,7 +22899,7 @@
         <v>9</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -22928,7 +22928,7 @@
         <v>6</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -23073,7 +23073,7 @@
         <v>9</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -23102,7 +23102,7 @@
         <v>6</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -23247,7 +23247,7 @@
         <v>9</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -23276,7 +23276,7 @@
         <v>6</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -23421,7 +23421,7 @@
         <v>9</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -23450,7 +23450,7 @@
         <v>6</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -23595,7 +23595,7 @@
         <v>9</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -23624,7 +23624,7 @@
         <v>6</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -23769,7 +23769,7 @@
         <v>9</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -23798,7 +23798,7 @@
         <v>6</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -23943,7 +23943,7 @@
         <v>9</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -23972,7 +23972,7 @@
         <v>6</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -24117,7 +24117,7 @@
         <v>9</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -24146,7 +24146,7 @@
         <v>6</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -24291,7 +24291,7 @@
         <v>9</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -24320,7 +24320,7 @@
         <v>6</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -24465,7 +24465,7 @@
         <v>9</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -24494,7 +24494,7 @@
         <v>6</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -24639,7 +24639,7 @@
         <v>9</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -24668,7 +24668,7 @@
         <v>6</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -24813,7 +24813,7 @@
         <v>9</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -24842,7 +24842,7 @@
         <v>6</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -24987,7 +24987,7 @@
         <v>9</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -25016,7 +25016,7 @@
         <v>6</v>
       </c>
       <c r="I139" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -25161,7 +25161,7 @@
         <v>9</v>
       </c>
       <c r="I144" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -25190,7 +25190,7 @@
         <v>6</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -25335,7 +25335,7 @@
         <v>9</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -25364,7 +25364,7 @@
         <v>6</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -25509,7 +25509,7 @@
         <v>9</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -25538,7 +25538,7 @@
         <v>6</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -26404,7 +26404,7 @@
       </c>
       <c r="I186" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>T1</v>
+        <v>T2</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -26438,7 +26438,7 @@
       </c>
       <c r="I187" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>T1</v>
+        <v>T2</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -26608,7 +26608,7 @@
       </c>
       <c r="I192" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>T1</v>
+        <v>T2</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -26642,7 +26642,7 @@
       </c>
       <c r="I193" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>T1</v>
+        <v>T2</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -26797,7 +26797,7 @@
       </c>
       <c r="I198" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>T1</v>
+        <v>T2</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -26828,7 +26828,7 @@
       </c>
       <c r="I199" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>T1</v>
+        <v>T2</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -26983,7 +26983,7 @@
       </c>
       <c r="I204" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>T1</v>
+        <v>T2</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -27014,7 +27014,7 @@
       </c>
       <c r="I205" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>T1</v>
+        <v>T2</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -27159,7 +27159,7 @@
         <v>9</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -27188,7 +27188,7 @@
         <v>6</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -27333,7 +27333,7 @@
         <v>9</v>
       </c>
       <c r="I216" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -27362,7 +27362,7 @@
         <v>6</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -27507,7 +27507,7 @@
         <v>9</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -27536,7 +27536,7 @@
         <v>6</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -27681,7 +27681,7 @@
         <v>9</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -27710,7 +27710,7 @@
         <v>6</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -29144,12 +29144,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29323,15 +29320,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29355,17 +29363,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Extract INTERNAL_LOADS and INDOOR_COMFORT to use_types"
This reverts commit 0de86661edcaa0f669faa81b56f5d2ff3f6309b9.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/construction_properties.xlsx
+++ b/cea/databases/CH/archetypes/construction_properties.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2930" windowWidth="19340" windowHeight="16460" tabRatio="785" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2925" windowWidth="19335" windowHeight="16455" tabRatio="785"/>
   </bookViews>
   <sheets>
     <sheet name="ARCHITECTURE" sheetId="3" r:id="rId1"/>
     <sheet name="AIR_CONDITIONING" sheetId="1" r:id="rId2"/>
     <sheet name="SUPPLY" sheetId="8" r:id="rId3"/>
     <sheet name="EMISSION_INTENSITY" sheetId="9" r:id="rId4"/>
+    <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId5"/>
+    <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="107">
+  <si>
+    <t>Code</t>
+  </si>
   <si>
     <t>type_hs</t>
   </si>
@@ -62,6 +67,75 @@
     <t>T4</t>
   </si>
   <si>
+    <t>Ths_set_C</t>
+  </si>
+  <si>
+    <t>Ea_Wm2</t>
+  </si>
+  <si>
+    <t>El_Wm2</t>
+  </si>
+  <si>
+    <t>Epro_Wm2</t>
+  </si>
+  <si>
+    <t>Tcs_set_C</t>
+  </si>
+  <si>
+    <t>MULTI_RES</t>
+  </si>
+  <si>
+    <t>SINGLE_RES</t>
+  </si>
+  <si>
+    <t>HOTEL</t>
+  </si>
+  <si>
+    <t>OFFICE</t>
+  </si>
+  <si>
+    <t>RETAIL</t>
+  </si>
+  <si>
+    <t>RESTAURANT</t>
+  </si>
+  <si>
+    <t>INDUSTRIAL</t>
+  </si>
+  <si>
+    <t>SCHOOL</t>
+  </si>
+  <si>
+    <t>HOSPITAL</t>
+  </si>
+  <si>
+    <t>GYM</t>
+  </si>
+  <si>
+    <t>SWIMMING</t>
+  </si>
+  <si>
+    <t>SERVERROOM</t>
+  </si>
+  <si>
+    <t>PARKING</t>
+  </si>
+  <si>
+    <t>COOLROOM</t>
+  </si>
+  <si>
+    <t>FOODSTORE</t>
+  </si>
+  <si>
+    <t>Ed_Wm2</t>
+  </si>
+  <si>
+    <t>Tcs_setb_C</t>
+  </si>
+  <si>
+    <t>Ths_setb_C</t>
+  </si>
+  <si>
     <t>type_win</t>
   </si>
   <si>
@@ -77,6 +151,15 @@
     <t>type_vent</t>
   </si>
   <si>
+    <t>LAB</t>
+  </si>
+  <si>
+    <t>MUSEUM</t>
+  </si>
+  <si>
+    <t>LIBRARY</t>
+  </si>
+  <si>
     <t>T6</t>
   </si>
   <si>
@@ -119,6 +202,9 @@
     <t>year_end</t>
   </si>
   <si>
+    <t>Qhpro_Wm2</t>
+  </si>
+  <si>
     <t>wwr_north</t>
   </si>
   <si>
@@ -137,10 +223,43 @@
     <t>type_el</t>
   </si>
   <si>
+    <t>Qcre_Wm2</t>
+  </si>
+  <si>
     <t>Ns</t>
   </si>
   <si>
     <t>Es</t>
+  </si>
+  <si>
+    <t>UNIVERSITY</t>
+  </si>
+  <si>
+    <t>Qcpro_Wm2</t>
+  </si>
+  <si>
+    <t>Occ_m2pax</t>
+  </si>
+  <si>
+    <t>Vww_lpdpax</t>
+  </si>
+  <si>
+    <t>Vw_lpdpax</t>
+  </si>
+  <si>
+    <t>X_ghpax</t>
+  </si>
+  <si>
+    <t>Qs_Wpax</t>
+  </si>
+  <si>
+    <t>Ve_lpspax</t>
+  </si>
+  <si>
+    <t>RH_min_pc</t>
+  </si>
+  <si>
+    <t>RH_max_pc</t>
   </si>
   <si>
     <t>16|09</t>
@@ -572,7 +691,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -702,6 +821,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -747,7 +879,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -756,7 +888,14 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -767,6 +906,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1130,108 +1276,186 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2019-08-09T09:30:43.03" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{4995A51A-970E-4858-A3E9-F23AAFC3B2D7}">
+    <text>do not find this in SIA</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2019-08-13T15:04:41.29" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{59FCE18A-D39A-4487-B53C-3197D510A233}" parentId="{4995A51A-970E-4858-A3E9-F23AAFC3B2D7}">
+    <text>keep the same as old CEA Databases
+!</text>
+  </threadedComment>
+  <threadedComment ref="F14" dT="2019-08-13T15:40:02.18" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{19AF7AA5-1871-49D1-8FCF-02DD9C759BA1}">
+    <text>do not change from old CEA database</text>
+  </threadedComment>
+  <threadedComment ref="G15" dT="2019-08-13T14:54:06.63" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{1E62239D-37F6-4696-B130-748547BDA1A6}">
+    <text>nothing in SIA</text>
+  </threadedComment>
+  <threadedComment ref="G15" dT="2019-08-14T15:42:57.84" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{16CCDA4D-D51F-44AA-95EC-8AE62BEBEB94}" parentId="{1E62239D-37F6-4696-B130-748547BDA1A6}">
+    <text>Keep same as old CEA database
+These are not used anyway for these building typologies</text>
+  </threadedComment>
+  <threadedComment ref="G16" dT="2019-08-13T14:52:59.52" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{CB14F6D7-71C4-4A0D-B956-D1AB18BB535B}">
+    <text>nothing in SIA 2024</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F1" dT="2019-08-08T12:20:45.51" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{2BD16210-01D2-42DE-9F57-124A6EE12ECA}">
+    <text>dont find in SIA</text>
+  </threadedComment>
+  <threadedComment ref="F1" dT="2019-08-13T08:16:02.08" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{6906B04C-56FB-4FF5-BF02-6B67D8F3AD90}" parentId="{2BD16210-01D2-42DE-9F57-124A6EE12ECA}">
+    <text>kept same as old CEA database - no reference available to change these values</text>
+  </threadedComment>
+  <threadedComment ref="G1" dT="2019-08-08T12:23:57.13" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{2ED044A9-C68D-45BD-B13C-0553F43D3768}">
+    <text>dont find in SIA</text>
+  </threadedComment>
+  <threadedComment ref="J1" dT="2019-08-08T12:08:25.79" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{4188EAE4-5F6C-4CB7-96DC-907AA428BC99}">
+    <text>cannot find in SIA</text>
+  </threadedComment>
+  <threadedComment ref="J1" dT="2019-08-13T12:13:58.38" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{F1EF6245-8799-47A6-BCFF-35017E08DD5E}" parentId="{4188EAE4-5F6C-4CB7-96DC-907AA428BC99}">
+    <text>no other source available - keep same as in old CEA database</text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2019-08-08T12:08:53.23" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{31840D2C-BF6D-496C-92D3-7147ADE02D81}">
+    <text>no reference available - keep same as in old CEA database</text>
+  </threadedComment>
+  <threadedComment ref="A4" dT="2019-08-08T15:02:30.20" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{BA522695-9F5A-4685-BC9C-BB455B175508}">
+    <text>hotelzimmer values used</text>
+  </threadedComment>
+  <threadedComment ref="A5" dT="2019-08-08T15:03:11.08" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{AB79D271-718E-45F1-9D6A-2D1684E778DD}">
+    <text>einzel/gruppenburo values used</text>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2019-08-08T15:03:58.66" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{99BBF83B-3C08-41AC-84FA-45BAB926754C}">
+    <text>fachgeschaft</text>
+  </threadedComment>
+  <threadedComment ref="A7" dT="2019-08-08T15:04:09.18" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{2E89370B-2C8B-441B-8524-4961F9AD1E21}">
+    <text>lebensmittelverkauf = supermarket</text>
+  </threadedComment>
+  <threadedComment ref="A9" dT="2019-08-08T15:05:24.19" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{10829547-C2A4-4E58-B632-CF7EDF7CE835}">
+    <text>grosse arbeit values are used</text>
+  </threadedComment>
+  <threadedComment ref="A10" dT="2019-08-08T15:08:09.77" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{139CF0AD-AE2C-4F6B-9B40-AE63022A2B59}">
+    <text>schulzimmer values</text>
+  </threadedComment>
+  <threadedComment ref="A11" dT="2019-08-08T14:52:31.15" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{EB7016A0-8719-4E80-9845-07E465C0EED2}">
+    <text>do not know which one to take - 3 categories of rooms are available</text>
+  </threadedComment>
+  <threadedComment ref="A11" dT="2019-08-13T12:21:38.00" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{A96F6928-49E1-45C2-8A9F-9831A5C098A7}" parentId="{EB7016A0-8719-4E80-9845-07E465C0EED2}">
+    <text>all values from Bettenzimmer SIA 2024 8.1</text>
+  </threadedComment>
+  <threadedComment ref="F17" dT="2019-08-13T08:16:17.03" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{74014532-D18F-4AA9-A13E-1879A8CF80D5}">
+    <text>same as industrial</text>
+  </threadedComment>
+  <threadedComment ref="A20" dT="2019-08-08T14:58:20.10" personId="{CCCC8246-769A-4BF8-9848-A321DBADB4A3}" id="{4A6E4AE9-26FD-441F-92BA-0F9C18F35B56}">
+    <text>Horsaal is taken for this</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.54296875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" style="3" customWidth="1"/>
-    <col min="12" max="13" width="10.81640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="11.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="12.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.1796875" style="1"/>
+    <col min="11" max="11" width="11.5703125" style="3" customWidth="1"/>
+    <col min="12" max="13" width="10.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="J1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="S1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="22">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="18">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>18</v>
       </c>
       <c r="E2" s="2">
         <v>0.82</v>
@@ -1242,10 +1466,10 @@
       <c r="G2" s="2">
         <v>0.82</v>
       </c>
-      <c r="H2" s="9">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8">
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10">
         <v>0</v>
       </c>
       <c r="J2" s="2">
@@ -1261,37 +1485,37 @@
         <v>0.16</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" s="6"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="T2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="E3" s="2">
         <v>0.82</v>
@@ -1302,10 +1526,10 @@
       <c r="G3" s="2">
         <v>0.82</v>
       </c>
-      <c r="H3" s="9">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
         <v>0</v>
       </c>
       <c r="J3" s="2">
@@ -1321,37 +1545,37 @@
         <v>0.21</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="T3" s="6"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>23</v>
+      <c r="B4" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="E4" s="2">
         <v>0.82</v>
@@ -1362,10 +1586,10 @@
       <c r="G4" s="2">
         <v>0.82</v>
       </c>
-      <c r="H4" s="9">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8">
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10">
         <v>0</v>
       </c>
       <c r="J4" s="2">
@@ -1381,37 +1605,37 @@
         <v>0.25</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="T4" s="6"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="T4" s="8"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="E5" s="2">
         <v>0.82</v>
@@ -1422,10 +1646,10 @@
       <c r="G5" s="2">
         <v>0.82</v>
       </c>
-      <c r="H5" s="9">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
         <v>0</v>
       </c>
       <c r="J5" s="2">
@@ -1441,37 +1665,37 @@
         <v>0.21</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="T5" s="6"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="T5" s="8"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="E6" s="2">
         <v>0.82</v>
@@ -1482,10 +1706,10 @@
       <c r="G6" s="2">
         <v>0.82</v>
       </c>
-      <c r="H6" s="9">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
         <v>0</v>
       </c>
       <c r="J6" s="2">
@@ -1501,36 +1725,36 @@
         <v>0.15</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="E7" s="2">
         <v>0.82</v>
@@ -1541,10 +1765,10 @@
       <c r="G7" s="2">
         <v>0.82</v>
       </c>
-      <c r="H7" s="9">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="10">
         <v>0</v>
       </c>
       <c r="J7" s="2">
@@ -1560,22 +1784,22 @@
         <v>0.15</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1598,242 +1822,242 @@
       <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="12.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1850,133 +2074,133 @@
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="10" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E1" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1988,313 +2212,313 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="14" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.26953125" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.26953125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="13"/>
+    <col min="1" max="1" width="13.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="18" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="14">
         <v>57</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="17" t="s">
+      <c r="C2" s="14">
+        <v>57</v>
+      </c>
+      <c r="D2" s="14">
+        <v>39</v>
+      </c>
+      <c r="E2" s="14">
+        <v>32</v>
+      </c>
+      <c r="F2" s="14">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="G2" s="14">
+        <v>64</v>
+      </c>
+      <c r="H2" s="14">
+        <v>39</v>
+      </c>
+      <c r="I2" s="14">
+        <v>29</v>
+      </c>
+      <c r="J2" s="14">
+        <v>32</v>
+      </c>
+      <c r="K2" s="14">
+        <v>135</v>
+      </c>
+      <c r="L2" s="16">
+        <v>16</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14">
+        <v>34</v>
+      </c>
+      <c r="C3" s="14">
+        <v>34</v>
+      </c>
+      <c r="D3" s="14">
+        <v>32</v>
+      </c>
+      <c r="E3" s="14">
+        <v>20</v>
+      </c>
+      <c r="F3" s="14">
+        <v>62</v>
+      </c>
+      <c r="G3" s="14">
+        <v>113</v>
+      </c>
+      <c r="H3" s="14">
+        <v>113</v>
+      </c>
+      <c r="I3" s="14">
+        <v>57</v>
+      </c>
+      <c r="J3" s="14">
+        <v>32</v>
+      </c>
+      <c r="K3" s="14">
+        <v>135</v>
+      </c>
+      <c r="L3" s="16">
+        <v>16</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B4" s="14">
+        <v>36</v>
+      </c>
+      <c r="C4" s="14">
+        <v>35</v>
+      </c>
+      <c r="D4" s="14">
+        <v>34</v>
+      </c>
+      <c r="E4" s="14">
+        <v>21</v>
+      </c>
+      <c r="F4" s="14">
+        <v>123</v>
+      </c>
+      <c r="G4" s="14">
+        <v>110</v>
+      </c>
+      <c r="H4" s="14">
+        <v>113</v>
+      </c>
+      <c r="I4" s="14">
+        <v>113</v>
+      </c>
+      <c r="J4" s="14">
+        <v>32</v>
+      </c>
+      <c r="K4" s="14">
+        <v>135</v>
+      </c>
+      <c r="L4" s="16">
+        <v>16</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="14">
         <v>57</v>
       </c>
-      <c r="C2" s="10">
-        <v>57</v>
-      </c>
-      <c r="D2" s="10">
-        <v>39</v>
-      </c>
-      <c r="E2" s="10">
+      <c r="C5" s="14">
+        <v>71</v>
+      </c>
+      <c r="D5" s="14">
+        <v>34</v>
+      </c>
+      <c r="E5" s="14">
+        <v>21</v>
+      </c>
+      <c r="F5" s="14">
+        <v>69</v>
+      </c>
+      <c r="G5" s="14">
+        <v>91</v>
+      </c>
+      <c r="H5" s="14">
+        <v>104</v>
+      </c>
+      <c r="I5" s="14">
+        <v>113</v>
+      </c>
+      <c r="J5" s="14">
         <v>32</v>
       </c>
-      <c r="F2" s="10">
-        <v>47</v>
-      </c>
-      <c r="G2" s="10">
-        <v>64</v>
-      </c>
-      <c r="H2" s="10">
-        <v>39</v>
-      </c>
-      <c r="I2" s="10">
-        <v>29</v>
-      </c>
-      <c r="J2" s="10">
+      <c r="K5" s="14">
+        <v>135</v>
+      </c>
+      <c r="L5" s="16">
+        <v>16</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="14">
+        <v>112</v>
+      </c>
+      <c r="C6" s="14">
+        <v>188</v>
+      </c>
+      <c r="D6" s="14">
+        <v>73</v>
+      </c>
+      <c r="E6" s="14">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14">
+        <v>85</v>
+      </c>
+      <c r="G6" s="14">
+        <v>75</v>
+      </c>
+      <c r="H6" s="14">
+        <v>180</v>
+      </c>
+      <c r="I6" s="14">
+        <v>78</v>
+      </c>
+      <c r="J6" s="14">
         <v>32</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K6" s="14">
         <v>135</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L6" s="16">
         <v>16</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10">
-        <v>34</v>
-      </c>
-      <c r="C3" s="10">
-        <v>34</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="M6" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="14">
+        <v>112</v>
+      </c>
+      <c r="C7" s="14">
+        <v>188</v>
+      </c>
+      <c r="D7" s="14">
+        <v>73</v>
+      </c>
+      <c r="E7" s="14">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14">
+        <v>85</v>
+      </c>
+      <c r="G7" s="14">
+        <v>75</v>
+      </c>
+      <c r="H7" s="14">
+        <v>180</v>
+      </c>
+      <c r="I7" s="14">
+        <v>78</v>
+      </c>
+      <c r="J7" s="14">
         <v>32</v>
       </c>
-      <c r="E3" s="10">
-        <v>20</v>
-      </c>
-      <c r="F3" s="10">
-        <v>62</v>
-      </c>
-      <c r="G3" s="10">
-        <v>113</v>
-      </c>
-      <c r="H3" s="10">
-        <v>113</v>
-      </c>
-      <c r="I3" s="10">
-        <v>57</v>
-      </c>
-      <c r="J3" s="10">
-        <v>32</v>
-      </c>
-      <c r="K3" s="10">
+      <c r="K7" s="14">
         <v>135</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L7" s="16">
         <v>16</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="10">
-        <v>36</v>
-      </c>
-      <c r="C4" s="10">
-        <v>35</v>
-      </c>
-      <c r="D4" s="10">
-        <v>34</v>
-      </c>
-      <c r="E4" s="10">
-        <v>21</v>
-      </c>
-      <c r="F4" s="10">
-        <v>123</v>
-      </c>
-      <c r="G4" s="10">
-        <v>110</v>
-      </c>
-      <c r="H4" s="10">
-        <v>113</v>
-      </c>
-      <c r="I4" s="10">
-        <v>113</v>
-      </c>
-      <c r="J4" s="10">
-        <v>32</v>
-      </c>
-      <c r="K4" s="10">
-        <v>135</v>
-      </c>
-      <c r="L4" s="12">
-        <v>16</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="10">
-        <v>57</v>
-      </c>
-      <c r="C5" s="10">
-        <v>71</v>
-      </c>
-      <c r="D5" s="10">
-        <v>34</v>
-      </c>
-      <c r="E5" s="10">
-        <v>21</v>
-      </c>
-      <c r="F5" s="10">
-        <v>69</v>
-      </c>
-      <c r="G5" s="10">
-        <v>91</v>
-      </c>
-      <c r="H5" s="10">
-        <v>104</v>
-      </c>
-      <c r="I5" s="10">
-        <v>113</v>
-      </c>
-      <c r="J5" s="10">
-        <v>32</v>
-      </c>
-      <c r="K5" s="10">
-        <v>135</v>
-      </c>
-      <c r="L5" s="12">
-        <v>16</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="10">
-        <v>112</v>
-      </c>
-      <c r="C6" s="10">
-        <v>188</v>
-      </c>
-      <c r="D6" s="10">
-        <v>73</v>
-      </c>
-      <c r="E6" s="10">
-        <v>16</v>
-      </c>
-      <c r="F6" s="10">
-        <v>85</v>
-      </c>
-      <c r="G6" s="10">
-        <v>75</v>
-      </c>
-      <c r="H6" s="10">
-        <v>180</v>
-      </c>
-      <c r="I6" s="10">
-        <v>78</v>
-      </c>
-      <c r="J6" s="10">
-        <v>32</v>
-      </c>
-      <c r="K6" s="10">
-        <v>135</v>
-      </c>
-      <c r="L6" s="12">
-        <v>16</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="10">
-        <v>112</v>
-      </c>
-      <c r="C7" s="10">
-        <v>188</v>
-      </c>
-      <c r="D7" s="10">
-        <v>73</v>
-      </c>
-      <c r="E7" s="10">
-        <v>16</v>
-      </c>
-      <c r="F7" s="10">
-        <v>85</v>
-      </c>
-      <c r="G7" s="10">
-        <v>75</v>
-      </c>
-      <c r="H7" s="10">
-        <v>180</v>
-      </c>
-      <c r="I7" s="10">
-        <v>78</v>
-      </c>
-      <c r="J7" s="10">
-        <v>32</v>
-      </c>
-      <c r="K7" s="10">
-        <v>135</v>
-      </c>
-      <c r="L7" s="12">
-        <v>16</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>48</v>
+      <c r="M7" s="15" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2303,13 +2527,1437 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="13">
+        <v>30</v>
+      </c>
+      <c r="C2" s="13">
+        <v>70</v>
+      </c>
+      <c r="D2" s="13">
+        <v>80</v>
+      </c>
+      <c r="E2" s="13">
+        <v>8</v>
+      </c>
+      <c r="F2" s="13">
+        <v>2.7</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13">
+        <v>35</v>
+      </c>
+      <c r="J2" s="13">
+        <v>140</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0</v>
+      </c>
+      <c r="L2" s="11">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="13">
+        <v>50</v>
+      </c>
+      <c r="C3" s="11">
+        <v>70</v>
+      </c>
+      <c r="D3" s="11">
+        <v>80</v>
+      </c>
+      <c r="E3" s="11">
+        <v>8</v>
+      </c>
+      <c r="F3" s="11">
+        <v>2.7</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>40</v>
+      </c>
+      <c r="J3" s="13">
+        <v>160</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11">
+        <v>0</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="13">
+        <v>15</v>
+      </c>
+      <c r="C4" s="13">
+        <v>70</v>
+      </c>
+      <c r="D4" s="13">
+        <v>80</v>
+      </c>
+      <c r="E4" s="13">
+        <v>8</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2.7</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
+        <v>40</v>
+      </c>
+      <c r="J4" s="13">
+        <v>160</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="13">
+        <v>14</v>
+      </c>
+      <c r="C5" s="13">
+        <v>70</v>
+      </c>
+      <c r="D5" s="13">
+        <v>80</v>
+      </c>
+      <c r="E5" s="13">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13">
+        <v>15.9</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13">
+        <v>3</v>
+      </c>
+      <c r="J5" s="13">
+        <v>60</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="13">
+        <v>8</v>
+      </c>
+      <c r="C6" s="13">
+        <v>70</v>
+      </c>
+      <c r="D6" s="13">
+        <v>80</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2</v>
+      </c>
+      <c r="F6" s="13">
+        <f>9.3+24</f>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
+        <v>2</v>
+      </c>
+      <c r="J6" s="13">
+        <v>30</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="13">
+        <v>8</v>
+      </c>
+      <c r="C7" s="13">
+        <v>70</v>
+      </c>
+      <c r="D7" s="13">
+        <v>80</v>
+      </c>
+      <c r="E7" s="13">
+        <v>2</v>
+      </c>
+      <c r="F7" s="13">
+        <f>9.3+12</f>
+        <v>21.3</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
+        <v>2</v>
+      </c>
+      <c r="J7" s="13">
+        <v>30</v>
+      </c>
+      <c r="K7" s="11">
+        <v>10</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="13">
+        <v>2</v>
+      </c>
+      <c r="C8" s="13">
+        <v>70</v>
+      </c>
+      <c r="D8" s="13">
+        <v>80</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2</v>
+      </c>
+      <c r="F8" s="13">
+        <v>6.9</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>15</v>
+      </c>
+      <c r="J8" s="13">
+        <v>45</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="13">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13">
+        <v>90</v>
+      </c>
+      <c r="D9" s="13">
+        <v>170</v>
+      </c>
+      <c r="E9" s="13">
+        <v>10</v>
+      </c>
+      <c r="F9" s="13">
+        <v>10.8</v>
+      </c>
+      <c r="G9" s="13">
+        <v>16.5</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
+        <v>3</v>
+      </c>
+      <c r="J9" s="13">
+        <v>60</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
+        <v>150</v>
+      </c>
+      <c r="M9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="13">
+        <v>3</v>
+      </c>
+      <c r="C10" s="13">
+        <v>70</v>
+      </c>
+      <c r="D10" s="13">
+        <v>80</v>
+      </c>
+      <c r="E10" s="13">
+        <v>4</v>
+      </c>
+      <c r="F10" s="13">
+        <v>14</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
+        <v>2</v>
+      </c>
+      <c r="J10" s="13">
+        <v>30</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0</v>
+      </c>
+      <c r="M10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="13">
+        <f>15*0.43+3*0.01+5*0.56</f>
+        <v>9.2800000000000011</v>
+      </c>
+      <c r="C11" s="13">
+        <v>70</v>
+      </c>
+      <c r="D11" s="13">
+        <v>80</v>
+      </c>
+      <c r="E11" s="13">
+        <f>0.43*4+0.01*7+0.56*20</f>
+        <v>12.990000000000002</v>
+      </c>
+      <c r="F11" s="13">
+        <f>0.43*4.5+0.01*15.9+0.56*15.9</f>
+        <v>10.998000000000001</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
+        <f>0.43*60+0.01*0+0.56*0</f>
+        <v>25.8</v>
+      </c>
+      <c r="J11" s="13">
+        <f>I11*4</f>
+        <v>103.2</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11">
+        <v>16</v>
+      </c>
+      <c r="M11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="13">
+        <v>10</v>
+      </c>
+      <c r="C12" s="13">
+        <v>120</v>
+      </c>
+      <c r="D12" s="13">
+        <v>280</v>
+      </c>
+      <c r="E12" s="13">
+        <v>2</v>
+      </c>
+      <c r="F12" s="13">
+        <v>9.9</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <v>60</v>
+      </c>
+      <c r="J12" s="13">
+        <v>180</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0</v>
+      </c>
+      <c r="M12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="13">
+        <v>70</v>
+      </c>
+      <c r="D13" s="13">
+        <v>80</v>
+      </c>
+      <c r="E13" s="13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="13">
+        <v>11.3</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
+        <v>120</v>
+      </c>
+      <c r="J13" s="13">
+        <v>360</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0</v>
+      </c>
+      <c r="C14" s="13">
+        <v>70</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>6.6</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>100</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="13">
+        <v>0</v>
+      </c>
+      <c r="C15" s="13">
+        <v>35</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
+        <v>2.9</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0</v>
+      </c>
+      <c r="M15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="13">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
+        <v>70</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0</v>
+      </c>
+      <c r="F16" s="13">
+        <v>5.7</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="13">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="11">
+        <v>100</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="M16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="13">
+        <v>15</v>
+      </c>
+      <c r="C17" s="13">
+        <f>C11</f>
+        <v>70</v>
+      </c>
+      <c r="D17" s="13">
+        <f>D11</f>
+        <v>80</v>
+      </c>
+      <c r="E17" s="13">
+        <v>20</v>
+      </c>
+      <c r="F17" s="13">
+        <v>16.2</v>
+      </c>
+      <c r="G17" s="13">
+        <f>G9</f>
+        <v>16.5</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="13">
+        <v>3</v>
+      </c>
+      <c r="J17" s="13">
+        <v>60</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="13">
+        <v>3</v>
+      </c>
+      <c r="C18" s="13">
+        <v>70</v>
+      </c>
+      <c r="D18" s="13">
+        <v>80</v>
+      </c>
+      <c r="E18" s="13">
+        <v>7</v>
+      </c>
+      <c r="F18" s="13">
+        <v>10.8</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="13">
+        <v>2</v>
+      </c>
+      <c r="J18" s="13">
+        <v>30</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0</v>
+      </c>
+      <c r="L18" s="11">
+        <v>0</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="13">
+        <v>5</v>
+      </c>
+      <c r="C19" s="13">
+        <v>70</v>
+      </c>
+      <c r="D19" s="13">
+        <v>80</v>
+      </c>
+      <c r="E19" s="13">
+        <v>2</v>
+      </c>
+      <c r="F19" s="13">
+        <v>6.9</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0</v>
+      </c>
+      <c r="H19" s="11">
+        <v>0</v>
+      </c>
+      <c r="I19" s="13">
+        <v>0</v>
+      </c>
+      <c r="J19" s="13">
+        <v>0</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0</v>
+      </c>
+      <c r="M19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="13">
+        <v>10</v>
+      </c>
+      <c r="C20" s="13">
+        <v>70</v>
+      </c>
+      <c r="D20" s="13">
+        <v>80</v>
+      </c>
+      <c r="E20" s="13">
+        <v>4</v>
+      </c>
+      <c r="F20" s="13">
+        <v>12.5</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="13">
+        <v>2</v>
+      </c>
+      <c r="J20" s="13">
+        <v>30</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11">
+        <v>0</v>
+      </c>
+      <c r="M20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4">
+        <v>18</v>
+      </c>
+      <c r="F2" s="11">
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="G2" s="11">
+        <v>30</v>
+      </c>
+      <c r="H2" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2">
+        <v>28</v>
+      </c>
+      <c r="E3" s="4">
+        <v>18</v>
+      </c>
+      <c r="F3" s="11">
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="G3" s="11">
+        <v>30</v>
+      </c>
+      <c r="H3" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4">
+        <v>21</v>
+      </c>
+      <c r="F4" s="11">
+        <f>36/3.6</f>
+        <v>10</v>
+      </c>
+      <c r="G4" s="11">
+        <v>30</v>
+      </c>
+      <c r="H4" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4">
+        <v>12</v>
+      </c>
+      <c r="F5" s="11">
+        <f>36/3.6</f>
+        <v>10</v>
+      </c>
+      <c r="G5" s="11">
+        <v>30</v>
+      </c>
+      <c r="H5" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>26</v>
+      </c>
+      <c r="C6" s="4">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4">
+        <v>12</v>
+      </c>
+      <c r="F6" s="11">
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="G6" s="11">
+        <v>30</v>
+      </c>
+      <c r="H6" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4">
+        <v>12</v>
+      </c>
+      <c r="F7" s="11">
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="G7" s="11">
+        <v>30</v>
+      </c>
+      <c r="H7" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4">
+        <v>12</v>
+      </c>
+      <c r="F8" s="11">
+        <f>36/3.6</f>
+        <v>10</v>
+      </c>
+      <c r="G8" s="11">
+        <v>30</v>
+      </c>
+      <c r="H8" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2">
+        <v>30</v>
+      </c>
+      <c r="C9" s="4">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2">
+        <v>32</v>
+      </c>
+      <c r="E9" s="4">
+        <v>12</v>
+      </c>
+      <c r="F9" s="11">
+        <f>10*15/3.6</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="G9" s="11">
+        <v>30</v>
+      </c>
+      <c r="H9" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2">
+        <v>28</v>
+      </c>
+      <c r="E10" s="4">
+        <v>12</v>
+      </c>
+      <c r="F10" s="11">
+        <f>25/3.6</f>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="G10" s="11">
+        <v>30</v>
+      </c>
+      <c r="H10" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4">
+        <v>21</v>
+      </c>
+      <c r="F11" s="11">
+        <f>36*1000/3600</f>
+        <v>10</v>
+      </c>
+      <c r="G11" s="11">
+        <v>30</v>
+      </c>
+      <c r="H11" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2">
+        <v>26</v>
+      </c>
+      <c r="C12" s="4">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2">
+        <v>28</v>
+      </c>
+      <c r="E12" s="4">
+        <v>12</v>
+      </c>
+      <c r="F12" s="11">
+        <f>9*10/3.6</f>
+        <v>25</v>
+      </c>
+      <c r="G12" s="11">
+        <v>30</v>
+      </c>
+      <c r="H12" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2">
+        <v>32</v>
+      </c>
+      <c r="E13" s="4">
+        <v>12</v>
+      </c>
+      <c r="F13" s="11">
+        <f>3.6*10/3.6</f>
+        <v>10</v>
+      </c>
+      <c r="G13" s="11">
+        <v>30</v>
+      </c>
+      <c r="H13" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2">
+        <v>28</v>
+      </c>
+      <c r="E14" s="4">
+        <v>12</v>
+      </c>
+      <c r="F14" s="11">
+        <v>36</v>
+      </c>
+      <c r="G14" s="11">
+        <v>30</v>
+      </c>
+      <c r="H14" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
+        <v>28</v>
+      </c>
+      <c r="E15" s="4">
+        <v>12</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>30</v>
+      </c>
+      <c r="H15" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>-18</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>30</v>
+      </c>
+      <c r="H16" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2">
+        <v>28</v>
+      </c>
+      <c r="E17" s="4">
+        <v>12</v>
+      </c>
+      <c r="F17" s="11">
+        <f>20*15/3.6</f>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="G17" s="11">
+        <v>30</v>
+      </c>
+      <c r="H17" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2">
+        <v>26</v>
+      </c>
+      <c r="C18" s="4">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4">
+        <v>12</v>
+      </c>
+      <c r="F18" s="11">
+        <f>36/3.6</f>
+        <v>10</v>
+      </c>
+      <c r="G18" s="11">
+        <v>30</v>
+      </c>
+      <c r="H18" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4">
+        <v>12</v>
+      </c>
+      <c r="F19" s="11">
+        <f>36/3.6</f>
+        <v>10</v>
+      </c>
+      <c r="G19" s="11">
+        <v>40</v>
+      </c>
+      <c r="H19" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2">
+        <v>26</v>
+      </c>
+      <c r="C20" s="4">
+        <v>21</v>
+      </c>
+      <c r="D20" s="2">
+        <v>28</v>
+      </c>
+      <c r="E20" s="4">
+        <v>12</v>
+      </c>
+      <c r="F20" s="11">
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="G20" s="11">
+        <v>30</v>
+      </c>
+      <c r="H20" s="11">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F2:F20" unlockedFormula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2483,15 +4131,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2515,17 +4174,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>